<commit_message>
Autamated Invalid Login with req excel data
</commit_message>
<xml_diff>
--- a/src/test/resources/data/input.xlsx
+++ b/src/test/resources/data/input.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>UserName</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Home Page Not Displayed</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -398,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -445,12 +451,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>